<commit_message>
afegit gestio dades i url de Actor
</commit_message>
<xml_diff>
--- a/pisos-sagrada_familia-2hab-2lav-con_aire-compra.xlsx
+++ b/pisos-sagrada_familia-2hab-2lav-con_aire-compra.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>430.000€</t>
+          <t>490.000€</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>490.000€</t>
+          <t>470.000€</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>470.000€</t>
+          <t>430.000€</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">

</xml_diff>

<commit_message>
paso per parametre url de Actor "start_urls"
</commit_message>
<xml_diff>
--- a/pisos-sagrada_familia-2hab-2lav-con_aire-compra.xlsx
+++ b/pisos-sagrada_familia-2hab-2lav-con_aire-compra.xlsx
@@ -592,7 +592,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>470.000€</t>
+          <t>430.000€</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>395.000€</t>
+          <t>470.000€</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>430.000€</t>
+          <t>395.000€</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">

</xml_diff>

<commit_message>
ficat el while request de la plantilla
</commit_message>
<xml_diff>
--- a/pisos-sagrada_familia-2hab-2lav-con_aire-compra.xlsx
+++ b/pisos-sagrada_familia-2hab-2lav-con_aire-compra.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>490.000€</t>
+          <t>470.000€</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>430.000€</t>
+          <t>395.000€</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>470.000€</t>
+          <t>490.000€</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>395.000€</t>
+          <t>430.000€</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">

</xml_diff>